<commit_message>
Deleted a lot of dead code, and refactored. Changed default behavior to show union of all rows which have an ID between two forms, as opposed to the intersection between the two.
</commit_message>
<xml_diff>
--- a/test/files/viffer/short/1.xlsx
+++ b/test/files/viffer/short/1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="26460" tabRatio="353"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15660" tabRatio="353"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -1620,7 +1620,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1628,8 +1628,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="253">
+  <cellStyleXfs count="255">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2387,8 +2407,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2473,8 +2499,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="253">
+  <cellStyles count="255">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -2600,6 +2632,7 @@
     <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -2725,6 +2758,7 @@
     <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 5" xfId="2"/>
@@ -3177,10 +3211,10 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0"/>
@@ -3206,7 +3240,7 @@
       <c r="D1" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="31" t="s">
         <v>10</v>
       </c>
       <c r="F1" s="25" t="s">
@@ -3276,7 +3310,7 @@
       <c r="J3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="25">
+      <c r="N3" s="30">
         <v>15002</v>
       </c>
     </row>

</xml_diff>